<commit_message>
update LAOs results, and fix small bugs
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [lab].xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [lab].xlsx
@@ -106,6 +106,12 @@
     <t>Total variable operating cost</t>
   </si>
   <si>
+    <t>Tridecane</t>
+  </si>
+  <si>
+    <t>CSL</t>
+  </si>
+  <si>
     <t>DAP</t>
   </si>
   <si>
@@ -119,12 +125,6 @@
   </si>
   <si>
     <t>Process water</t>
-  </si>
-  <si>
-    <t>Tridecane</t>
-  </si>
-  <si>
-    <t>CSL</t>
   </si>
   <si>
     <t>Natural gas</t>
@@ -528,7 +528,7 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>355.5815070353573</v>
+        <v>405.8710005627602</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -539,7 +539,7 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>66.54398004707662</v>
+        <v>62.47830084552534</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -550,7 +550,7 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>14.22326028141429</v>
+        <v>16.23484002251041</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -561,7 +561,7 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>32.00233563318216</v>
+        <v>36.52839005064841</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -572,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>16.00116781659108</v>
+        <v>18.26419502532421</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -583,7 +583,7 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>484.3522508136214</v>
+        <v>539.3767265067685</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -594,7 +594,7 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>48.43522508136215</v>
+        <v>53.93767265067685</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -605,7 +605,7 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>48.43522508136215</v>
+        <v>53.93767265067685</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -616,7 +616,7 @@
         <v>22</v>
       </c>
       <c r="C11">
-        <v>96.8704501627243</v>
+        <v>107.8753453013537</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="C12">
-        <v>145.3056752440864</v>
+        <v>161.8130179520305</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -638,7 +638,7 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>48.43522508136215</v>
+        <v>53.93767265067685</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -649,7 +649,7 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>387.4818006508973</v>
+        <v>431.5013812054149</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -660,7 +660,7 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>871.8340514645188</v>
+        <v>970.8781077121834</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -671,7 +671,7 @@
         <v>24</v>
       </c>
       <c r="C16">
-        <v>43.59170257322594</v>
+        <v>48.54390538560917</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -682,7 +682,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>915.4257540377447</v>
+        <v>1019.422013097793</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -701,10 +701,10 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>895.3915949999999</v>
+        <v>878.1550799999999</v>
       </c>
       <c r="D21">
-        <v>11.20645469371699</v>
+        <v>0.02944919024573181</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -713,10 +713,10 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>240.404025</v>
+        <v>51.528108</v>
       </c>
       <c r="D22">
-        <v>231.5793396277902</v>
+        <v>6.106799307209393</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -725,62 +725,62 @@
         <v>32</v>
       </c>
       <c r="C23">
-        <v>136.07775</v>
+        <v>895.3915949999999</v>
       </c>
       <c r="D23">
-        <v>40.22413798875953</v>
+        <v>14.44643600469633</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C24">
-        <v>-1.149733201553418</v>
+        <v>240.404025</v>
       </c>
       <c r="D24">
-        <v>-34.18704650491632</v>
+        <v>231.5793396277901</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>0.320236305</v>
+        <v>136.07775</v>
       </c>
       <c r="D25">
-        <v>9.463948228854406</v>
+        <v>51.8569443828605</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C26">
-        <v>878.1550799999999</v>
+        <v>-1.122754726231208</v>
       </c>
       <c r="D26">
-        <v>0.02284300215179679</v>
+        <v>-43.07057236753541</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C27">
-        <v>51.528108</v>
+        <v>0.320236305</v>
       </c>
       <c r="D27">
-        <v>4.764973215247072</v>
+        <v>12.20091644845022</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -792,7 +792,7 @@
         <v>197.76633</v>
       </c>
       <c r="D28">
-        <v>16.41288925306473</v>
+        <v>12.40122128402908</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -801,7 +801,7 @@
       </c>
       <c r="B29" s="1"/>
       <c r="D29">
-        <v>347.8616325145011</v>
+        <v>371.6916786128169</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -851,10 +851,10 @@
         <v>44</v>
       </c>
       <c r="C35">
-        <v>10.66744521106072</v>
+        <v>12.17613001688281</v>
       </c>
       <c r="D35">
-        <v>10.24074740261829</v>
+        <v>11.68908481620749</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -865,16 +865,16 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>2.489070549247501</v>
+        <v>2.841097003939321</v>
       </c>
       <c r="D36">
-        <v>2.389507727277601</v>
+        <v>2.727453123781749</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>